<commit_message>
fix: corregir typo en email de Roberto Madahuar (madahuar → rmadahuar)
- Corregido en FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx (filas 103-104)
- Email: madahuar@cotexsa.com.mx → rmadahuar@cotexsa.com.mx
- Credencial 115 sincronizado en Firebase
- Reportes RELACIÓN y ANEXO A regenerados
</commit_message>
<xml_diff>
--- a/data/reportes-bimestrales/2026/02/ANEXO_A_2026_02.xlsx
+++ b/data/reportes-bimestrales/2026/02/ANEXO_A_2026_02.xlsx
@@ -628,22 +628,22 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B7" t="str">
-        <v>humh4@hotmail.com</v>
+        <v>rmadahuar@cotexsa.com.mx</v>
       </c>
       <c r="C7" t="str">
-        <v>HUGO MARTINEZ HERNANDEZ</v>
+        <v>ROBERTO JOSE MADAHUAR BOEHM</v>
       </c>
       <c r="D7" t="str">
-        <v>9961006288</v>
+        <v>9999473478</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -663,25 +663,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B8" t="str">
-        <v>josebadz@outlook.com</v>
+        <v>humh4@hotmail.com</v>
       </c>
       <c r="C8" t="str">
-        <v>JOSE HIPOLITO BARRERA AKE</v>
+        <v>HUGO MARTINEZ HERNANDEZ</v>
       </c>
       <c r="D8" t="str">
-        <v>9818296516</v>
+        <v>9961006288</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -698,25 +698,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B9" t="str">
-        <v>cudaosj@hotmail.com</v>
+        <v>josebadz@outlook.com</v>
       </c>
       <c r="C9" t="str">
-        <v>ALEJANDRO JAVIER GARCÍA GAMBOA</v>
+        <v>JOSE HIPOLITO BARRERA AKE</v>
       </c>
       <c r="D9" t="str">
-        <v>9999001272</v>
+        <v>9818296516</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -733,28 +733,28 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B10" t="str">
-        <v>smunozam@gmail.com</v>
+        <v>cudaosj@hotmail.com</v>
       </c>
       <c r="C10" t="str">
-        <v>SERGIO MUÑOZ DE ALBA MEDRANO</v>
+        <v>ALEJANDRO JAVIER GARCÍA GAMBOA</v>
       </c>
       <c r="D10" t="str">
-        <v>9992005550</v>
+        <v>9999001272</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -768,31 +768,31 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B11" t="str">
-        <v>agm@galletasdonde.com</v>
+        <v>smunozam@gmail.com</v>
       </c>
       <c r="C11" t="str">
-        <v>ALEJANDRO GOMORY MARTINEZ</v>
+        <v>SERGIO MUÑOZ DE ALBA MEDRANO</v>
       </c>
       <c r="D11" t="str">
-        <v>9999490494</v>
+        <v>9992005550</v>
       </c>
       <c r="E11">
         <v>6</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="str">
         <v>N/A</v>
@@ -803,31 +803,31 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" t="str">
-        <v>javier_ruzperaza@hotmail.com</v>
+        <v>agm@galletasdonde.com</v>
       </c>
       <c r="C12" t="str">
-        <v>JAVIER RUZ PERAZA</v>
+        <v>ALEJANDRO GOMORY MARTINEZ</v>
       </c>
       <c r="D12" t="str">
-        <v>9992429052</v>
+        <v>9999490494</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="str">
         <v>N/A</v>
@@ -838,28 +838,28 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" t="str">
-        <v>hanstb@gmail.com</v>
+        <v>javier_ruzperaza@hotmail.com</v>
       </c>
       <c r="C13" t="str">
-        <v>HANS JURGEN THIES BARBACHANO</v>
+        <v>JAVIER RUZ PERAZA</v>
       </c>
       <c r="D13" t="str">
-        <v>9999415052</v>
+        <v>9992429052</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -873,86 +873,86 @@
     </row>
     <row r="14">
       <c r="A14">
+        <v>149</v>
+      </c>
+      <c r="B14" t="str">
+        <v>hanstb@gmail.com</v>
+      </c>
+      <c r="C14" t="str">
+        <v>HANS JURGEN THIES BARBACHANO</v>
+      </c>
+      <c r="D14" t="str">
+        <v>9999415052</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K14" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
         <v>151</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B15" t="str">
         <v>david_xolz@hotmail.com</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C15" t="str">
         <v>DAVID HOMERO SCHOLZ MORENO</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D15" t="str">
         <v>9999494819</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K14" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K15" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
         <v>153</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B16" t="str">
         <v>josegilbertohernandezcarrillo@gmail.com</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C16" t="str">
         <v>JOSE GILBERTO HERNANDEZ CARRILLO</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D16" t="str">
         <v>'9992389961</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K15" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>157</v>
-      </c>
-      <c r="B16" t="str">
-        <v>galvani@hotmail.com</v>
-      </c>
-      <c r="C16" t="str">
-        <v>EZEQUIEL GALVAN VAZQUEZ</v>
-      </c>
-      <c r="D16" t="str">
-        <v>9991335899</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -978,25 +978,25 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B17" t="str">
-        <v>agus_tin1_@hotmail.com</v>
+        <v>galvani@hotmail.com</v>
       </c>
       <c r="C17" t="str">
-        <v>AGUSTIN MORENO VILLALOBOS</v>
-      </c>
-      <c r="D17">
-        <v>9992780476</v>
+        <v>EZEQUIEL GALVAN VAZQUEZ</v>
+      </c>
+      <c r="D17" t="str">
+        <v>9991335899</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1013,28 +1013,28 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B18" t="str">
-        <v>rafael-rivas-p@hotmail.com</v>
+        <v>agus_tin1_@hotmail.com</v>
       </c>
       <c r="C18" t="str">
-        <v>RAFAEL RIVAS POLANCO</v>
-      </c>
-      <c r="D18" t="str">
-        <v>9999477501</v>
+        <v>AGUSTIN MORENO VILLALOBOS</v>
+      </c>
+      <c r="D18">
+        <v>9992780476</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1048,28 +1048,28 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" t="str">
-        <v>alejandrapintado@yahoo.com.mx</v>
+        <v>rafael-rivas-p@hotmail.com</v>
       </c>
       <c r="C19" t="str">
-        <v>ALEJANDRA GEORGINA PINTADO VILLAFAÑA</v>
+        <v>RAFAEL RIVAS POLANCO</v>
       </c>
       <c r="D19" t="str">
-        <v>9999479199</v>
+        <v>9999477501</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1083,16 +1083,16 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B20" t="str">
-        <v>tonysantacruz@hotmail.com</v>
+        <v>alejandrapintado@yahoo.com.mx</v>
       </c>
       <c r="C20" t="str">
-        <v>ANTONIO RAMÓN SANTA CRUZ POLANCO CABRALES</v>
+        <v>ALEJANDRA GEORGINA PINTADO VILLAFAÑA</v>
       </c>
       <c r="D20" t="str">
-        <v>9992243874</v>
+        <v>9999479199</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1101,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1118,16 +1118,16 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B21" t="str">
-        <v>marcotonyjr@hotmail.com</v>
+        <v>tonysantacruz@hotmail.com</v>
       </c>
       <c r="C21" t="str">
-        <v>MARCO ANTONIO SANTA CRUZ POLANCO CORDOVA</v>
+        <v>ANTONIO RAMÓN SANTA CRUZ POLANCO CABRALES</v>
       </c>
       <c r="D21" t="str">
-        <v>9992978103</v>
+        <v>9992243874</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1136,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1153,16 +1153,16 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B22" t="str">
-        <v>chafi70@hotmail.com</v>
+        <v>marcotonyjr@hotmail.com</v>
       </c>
       <c r="C22" t="str">
-        <v>CHAFI XACUR RIVERA</v>
+        <v>MARCO ANTONIO SANTA CRUZ POLANCO CORDOVA</v>
       </c>
       <c r="D22" t="str">
-        <v>9999477957</v>
+        <v>9992978103</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1188,28 +1188,28 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23" t="str">
-        <v>jcmaneo@hotmail.com</v>
+        <v>chafi70@hotmail.com</v>
       </c>
       <c r="C23" t="str">
-        <v>JUAN CARLOS MAÑE ORTIZ</v>
+        <v>CHAFI XACUR RIVERA</v>
       </c>
       <c r="D23" t="str">
-        <v>9991229424</v>
+        <v>9999477957</v>
       </c>
       <c r="E23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1223,28 +1223,28 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B24" t="str">
-        <v>tinosanchezf@yahoo.com.mx</v>
+        <v>jcmaneo@hotmail.com</v>
       </c>
       <c r="C24" t="str">
-        <v>CELESTINO SÁNCHEZ FERNÁNDEZ</v>
+        <v>JUAN CARLOS MAÑE ORTIZ</v>
       </c>
       <c r="D24" t="str">
-        <v>9992403110</v>
+        <v>9991229424</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1258,28 +1258,28 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B25" t="str">
-        <v>lalodenis23@hotmail.com</v>
+        <v>tinosanchezf@yahoo.com.mx</v>
       </c>
       <c r="C25" t="str">
-        <v>EDUARDO DENIS HERRERA</v>
+        <v>CELESTINO SÁNCHEZ FERNÁNDEZ</v>
       </c>
       <c r="D25" t="str">
-        <v>5520869685</v>
+        <v>9992403110</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1293,28 +1293,28 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B26" t="str">
-        <v>mayayuc3006@gmail.com</v>
+        <v>lalodenis23@hotmail.com</v>
       </c>
       <c r="C26" t="str">
-        <v>EDUARDO JOSE ARZAMENDI MONTEJO</v>
+        <v>EDUARDO DENIS HERRERA</v>
       </c>
       <c r="D26" t="str">
-        <v>9991276042</v>
+        <v>5520869685</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1328,25 +1328,25 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B27" t="str">
-        <v>rodrigo.garcia.e@live.com.mx</v>
+        <v>mayayuc3006@gmail.com</v>
       </c>
       <c r="C27" t="str">
-        <v>RODRIGO GARCÍA ESCALANTE</v>
+        <v>EDUARDO JOSE ARZAMENDI MONTEJO</v>
       </c>
       <c r="D27" t="str">
-        <v>9991375427</v>
+        <v>9991276042</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1363,28 +1363,28 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B28" t="str">
-        <v>jretana@live.com.mx</v>
+        <v>rodrigo.garcia.e@live.com.mx</v>
       </c>
       <c r="C28" t="str">
-        <v>JULIO RETANA VILLARREAL</v>
+        <v>RODRIGO GARCÍA ESCALANTE</v>
       </c>
       <c r="D28" t="str">
-        <v>9993356071</v>
+        <v>9991375427</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1398,25 +1398,25 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B29" t="str">
-        <v>d@azarcorp.mx</v>
+        <v>jretana@live.com.mx</v>
       </c>
       <c r="C29" t="str">
-        <v>DAVID AZAR CÁMARA</v>
+        <v>JULIO RETANA VILLARREAL</v>
       </c>
       <c r="D29" t="str">
-        <v>9991369874</v>
+        <v>9993356071</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1433,16 +1433,16 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" t="str">
-        <v>quiquis77@hotmail.com</v>
+        <v>d@azarcorp.mx</v>
       </c>
       <c r="C30" t="str">
-        <v>ENRIQUE GAONA CASTAÑEDA</v>
+        <v>DAVID AZAR CÁMARA</v>
       </c>
       <c r="D30" t="str">
-        <v>5520985073</v>
+        <v>9991369874</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1468,16 +1468,16 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" t="str">
-        <v>armando.pard@gmail.com</v>
+        <v>quiquis77@hotmail.com</v>
       </c>
       <c r="C31" t="str">
-        <v>ARMANDO PARDIÑAZ ALCANTARA</v>
+        <v>ENRIQUE GAONA CASTAÑEDA</v>
       </c>
       <c r="D31" t="str">
-        <v>9994992099</v>
+        <v>5520985073</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1503,28 +1503,28 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B32" t="str">
-        <v>jrgardoni@gmail.com</v>
+        <v>armando.pard@gmail.com</v>
       </c>
       <c r="C32" t="str">
-        <v>JOAQUIN RODOLFO GARDONI NUÑEZ</v>
+        <v>ARMANDO PARDIÑAZ ALCANTARA</v>
       </c>
       <c r="D32" t="str">
-        <v>5530565722</v>
+        <v>9994992099</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1538,28 +1538,28 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B33" t="str">
-        <v>valenciarojasjjesus@gmail.com</v>
+        <v>jrgardoni@gmail.com</v>
       </c>
       <c r="C33" t="str">
-        <v>J. JESÚS VALENCIA ROJAS</v>
+        <v>JOAQUIN RODOLFO GARDONI NUÑEZ</v>
       </c>
       <c r="D33" t="str">
-        <v>9971248940</v>
+        <v>5530565722</v>
       </c>
       <c r="E33">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -1573,28 +1573,28 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B34" t="str">
-        <v>brayerbyv@gmail.com</v>
+        <v>valenciarojasjjesus@gmail.com</v>
       </c>
       <c r="C34" t="str">
-        <v>BRAYER KERMITH VERDE CHIN</v>
+        <v>J. JESÚS VALENCIA ROJAS</v>
       </c>
       <c r="D34" t="str">
-        <v>9992247551</v>
+        <v>9971248940</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1608,31 +1608,31 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B35" t="str">
-        <v>rafle_30@hotmail.com</v>
+        <v>brayerbyv@gmail.com</v>
       </c>
       <c r="C35" t="str">
-        <v>ROGER IRÁN MÉNDEZ CARRILLO</v>
+        <v>BRAYER KERMITH VERDE CHIN</v>
       </c>
       <c r="D35" t="str">
-        <v>9991356502</v>
+        <v>9992247551</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="str">
         <v>N/A</v>
@@ -1643,31 +1643,31 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" t="str">
-        <v>mjtzab@yahoo.com</v>
+        <v>rafle_30@hotmail.com</v>
       </c>
       <c r="C36" t="str">
-        <v>MANUEL JESÚS TZAB CHUC</v>
+        <v>ROGER IRÁN MÉNDEZ CARRILLO</v>
       </c>
       <c r="D36" t="str">
-        <v>9991518266</v>
+        <v>9991356502</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="str">
         <v>N/A</v>
@@ -1678,16 +1678,16 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" t="str">
-        <v>lic.arielparedescetina@hotmail.com</v>
+        <v>mjtzab@yahoo.com</v>
       </c>
       <c r="C37" t="str">
-        <v>ARIEL ANTONIO PAREDES CETINA</v>
+        <v>MANUEL JESÚS TZAB CHUC</v>
       </c>
       <c r="D37" t="str">
-        <v>9994912883</v>
+        <v>9991518266</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1696,10 +1696,10 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -1713,28 +1713,28 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B38" t="str">
-        <v>dr.ricardocastillo@me.com</v>
+        <v>lic.arielparedescetina@hotmail.com</v>
       </c>
       <c r="C38" t="str">
-        <v>RICARDO ERNESTO CASTILLO MANCERA</v>
+        <v>ARIEL ANTONIO PAREDES CETINA</v>
       </c>
       <c r="D38" t="str">
-        <v>9901011913</v>
+        <v>9994912883</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -1748,28 +1748,28 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B39" t="str">
-        <v>cpedgardo_gomez@hotmail.com</v>
+        <v>dr.ricardocastillo@me.com</v>
       </c>
       <c r="C39" t="str">
-        <v>EDGARDO RAUL GÓMEZ ARZAMENDI</v>
+        <v>RICARDO ERNESTO CASTILLO MANCERA</v>
       </c>
       <c r="D39" t="str">
-        <v>9991450399</v>
+        <v>9901011913</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -1783,28 +1783,28 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B40" t="str">
-        <v>lolita@concepthaus.mx</v>
+        <v>cpedgardo_gomez@hotmail.com</v>
       </c>
       <c r="C40" t="str">
-        <v>MARIA DOLORES DAVIS BETANZOS</v>
+        <v>EDGARDO RAUL GÓMEZ ARZAMENDI</v>
       </c>
       <c r="D40" t="str">
-        <v>5543900616</v>
+        <v>9991450399</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -1818,25 +1818,25 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B41" t="str">
-        <v>santiago100100@hotmail.com</v>
+        <v>lolita@concepthaus.mx</v>
       </c>
       <c r="C41" t="str">
-        <v>SANTIAGO LAMAS RINGENBACH</v>
+        <v>MARIA DOLORES DAVIS BETANZOS</v>
       </c>
       <c r="D41" t="str">
-        <v>9993359825</v>
+        <v>5543900616</v>
       </c>
       <c r="E41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -1853,25 +1853,25 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B42" t="str">
-        <v>egpiccolo@gmail.com</v>
+        <v>santiago100100@hotmail.com</v>
       </c>
       <c r="C42" t="str">
-        <v>ERNESTO GONZALEZ PICCOLO</v>
+        <v>SANTIAGO LAMAS RINGENBACH</v>
       </c>
       <c r="D42" t="str">
-        <v>9995328570</v>
+        <v>9993359825</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -1888,16 +1888,16 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B43" t="str">
-        <v>arechiga@jogarplastics.com</v>
+        <v>egpiccolo@gmail.com</v>
       </c>
       <c r="C43" t="str">
-        <v>MARIA FERNANDA GUADALUPE ARECHIGA RAMOS</v>
+        <v>ERNESTO GONZALEZ PICCOLO</v>
       </c>
       <c r="D43" t="str">
-        <v>5537340096</v>
+        <v>9995328570</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -1906,10 +1906,10 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -1923,19 +1923,19 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B44" t="str">
-        <v>gfernandez63@gmail.com</v>
+        <v>arechiga@jogarplastics.com</v>
       </c>
       <c r="C44" t="str">
-        <v>GERARDO ANTONIO FERNÁNDEZ QUIJANO</v>
+        <v>MARIA FERNANDA GUADALUPE ARECHIGA RAMOS</v>
       </c>
       <c r="D44" t="str">
-        <v>9811204947</v>
+        <v>5537340096</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -1958,28 +1958,28 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B45" t="str">
-        <v>ridesquens@yahoo.com.mx</v>
+        <v>gfernandez63@gmail.com</v>
       </c>
       <c r="C45" t="str">
-        <v>RICARDO ALBERTO DESQUENS BONILLA</v>
+        <v>GERARDO ANTONIO FERNÁNDEZ QUIJANO</v>
       </c>
       <c r="D45" t="str">
-        <v>9993940909</v>
+        <v>9811204947</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -1993,28 +1993,28 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B46" t="str">
-        <v>martinezasergio@hotmail.com</v>
+        <v>ridesquens@yahoo.com.mx</v>
       </c>
       <c r="C46" t="str">
-        <v>SERGIO FERNANDO MARTINEZ AGUILAR</v>
+        <v>RICARDO ALBERTO DESQUENS BONILLA</v>
       </c>
       <c r="D46" t="str">
-        <v>9831549084</v>
+        <v>9993940909</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -2028,16 +2028,16 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B47" t="str">
-        <v>arobert01@protonmail.com</v>
+        <v>martinezasergio@hotmail.com</v>
       </c>
       <c r="C47" t="str">
-        <v>ALEJANDRO OLIVER ROBERT EASTMOND</v>
+        <v>SERGIO FERNANDO MARTINEZ AGUILAR</v>
       </c>
       <c r="D47" t="str">
-        <v>9999967145</v>
+        <v>9831549084</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -2046,10 +2046,10 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -2063,25 +2063,25 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B48" t="str">
-        <v>olga.garcia@mayaseguridad.mx</v>
+        <v>arobert01@protonmail.com</v>
       </c>
       <c r="C48" t="str">
-        <v>JUAN CARLOS RAMIREZ GOMEZ</v>
+        <v>ALEJANDRO OLIVER ROBERT EASTMOND</v>
       </c>
       <c r="D48" t="str">
-        <v>5543426160</v>
+        <v>9999967145</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -2098,19 +2098,19 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B49" t="str">
-        <v>gocaamal@hotmail.com</v>
+        <v>olga.garcia@mayaseguridad.mx</v>
       </c>
       <c r="C49" t="str">
-        <v>GADDI OTHONIEL CAAMAL PUC</v>
+        <v>JUAN CARLOS RAMIREZ GOMEZ</v>
       </c>
       <c r="D49" t="str">
-        <v>4431302953</v>
+        <v>5543426160</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -2133,19 +2133,19 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B50" t="str">
-        <v>guidorcuevasabraham@gmail.com</v>
+        <v>gocaamal@hotmail.com</v>
       </c>
       <c r="C50" t="str">
-        <v>GUIDO RENY CUEVAS ABRAHAM</v>
+        <v>GADDI OTHONIEL CAAMAL PUC</v>
       </c>
       <c r="D50" t="str">
-        <v>9993354270</v>
+        <v>4431302953</v>
       </c>
       <c r="E50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -2168,19 +2168,19 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B51" t="str">
-        <v>santiagorueda2@gmail.com</v>
+        <v>guidorcuevasabraham@gmail.com</v>
       </c>
       <c r="C51" t="str">
-        <v>SANTIAGO RUEDA ESCOBEDO</v>
+        <v>GUIDO RENY CUEVAS ABRAHAM</v>
       </c>
       <c r="D51" t="str">
-        <v>9381526811</v>
+        <v>9993354270</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2189,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -2203,28 +2203,28 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B52" t="str">
-        <v>ivancabo@gmail.com</v>
+        <v>santiagorueda2@gmail.com</v>
       </c>
       <c r="C52" t="str">
-        <v>IVAN TSUIS CABO TORRES</v>
+        <v>SANTIAGO RUEDA ESCOBEDO</v>
       </c>
       <c r="D52" t="str">
-        <v>9992315040</v>
+        <v>9381526811</v>
       </c>
       <c r="E52">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -2238,101 +2238,101 @@
     </row>
     <row r="53">
       <c r="A53">
+        <v>222</v>
+      </c>
+      <c r="B53" t="str">
+        <v>ivancabo@gmail.com</v>
+      </c>
+      <c r="C53" t="str">
+        <v>IVAN TSUIS CABO TORRES</v>
+      </c>
+      <c r="D53" t="str">
+        <v>9992315040</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K53" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
         <v>223</v>
       </c>
-      <c r="B53" t="str">
+      <c r="B54" t="str">
         <v>alejandro18sosa@gmail.com</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C54" t="str">
         <v>JESUS ALEJANDRO PUC SOSA</v>
       </c>
-      <c r="D53" t="str">
+      <c r="D54" t="str">
         <v>9993778311</v>
       </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-      <c r="J53" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K53" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K54" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
         <v>224</v>
       </c>
-      <c r="B54" t="str">
+      <c r="B55" t="str">
         <v>jgheredia@hotmail.com</v>
       </c>
-      <c r="C54" t="str">
+      <c r="C55" t="str">
         <v>JOSE GIL HEREDIA HAGAR</v>
       </c>
-      <c r="D54" t="str">
+      <c r="D55" t="str">
         <v>'9999001366</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>7</v>
       </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
         <v>5</v>
       </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-      <c r="J54" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K54" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>225</v>
-      </c>
-      <c r="B55" t="str">
-        <v>squintal158@gmail.com</v>
-      </c>
-      <c r="C55" t="str">
-        <v>SANTIAGO ALEJANDRO QUINTAL PAREDES</v>
-      </c>
-      <c r="D55" t="str">
-        <v>9995759542</v>
-      </c>
-      <c r="E55">
-        <v>3</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
-        <v>1</v>
-      </c>
-      <c r="H55">
-        <v>1</v>
-      </c>
       <c r="I55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="str">
         <v>N/A</v>
@@ -2343,28 +2343,28 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B56" t="str">
-        <v>atietzbabam@gmail.com</v>
+        <v>squintal158@gmail.com</v>
       </c>
       <c r="C56" t="str">
-        <v>ARIEL BALTAZAR CÓRDOBA WILSON</v>
+        <v>SANTIAGO ALEJANDRO QUINTAL PAREDES</v>
       </c>
       <c r="D56" t="str">
-        <v>9992003314</v>
+        <v>9995759542</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
       <c r="H56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -2378,28 +2378,28 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B57" t="str">
-        <v>ttok09136@gmail.com</v>
+        <v>atietzbabam@gmail.com</v>
       </c>
       <c r="C57" t="str">
-        <v>KRISZTIAN GOR</v>
+        <v>ARIEL BALTAZAR CÓRDOBA WILSON</v>
       </c>
       <c r="D57" t="str">
-        <v>+13213470270</v>
+        <v>9992003314</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -2413,28 +2413,28 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B58" t="str">
-        <v>fabian.sievers3548@gmail.com</v>
+        <v>ttok09136@gmail.com</v>
       </c>
       <c r="C58" t="str">
-        <v>FABIAN MARQUEZ ORTEGA</v>
+        <v>KRISZTIAN GOR</v>
       </c>
       <c r="D58" t="str">
-        <v>9993772793</v>
+        <v>+13213470270</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -2448,31 +2448,31 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B59" t="str">
-        <v>padilla_079@hotmail.com</v>
+        <v>fabian.sievers3548@gmail.com</v>
       </c>
       <c r="C59" t="str">
-        <v>DANIEL DE JESUS PADILLA ROBLES</v>
+        <v>FABIAN MARQUEZ ORTEGA</v>
       </c>
       <c r="D59" t="str">
-        <v>9991650849</v>
+        <v>9993772793</v>
       </c>
       <c r="E59">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F59">
         <v>1</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="str">
         <v>N/A</v>
@@ -2483,19 +2483,19 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B60" t="str">
-        <v>rsoberanis11@hotmail.com</v>
+        <v>padilla_079@hotmail.com</v>
       </c>
       <c r="C60" t="str">
-        <v>RICARDO ANTONIO SOBERANIS GAMBOA</v>
+        <v>DANIEL DE JESUS PADILLA ROBLES</v>
       </c>
       <c r="D60" t="str">
-        <v>9993437376</v>
+        <v>9991650849</v>
       </c>
       <c r="E60">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2504,10 +2504,10 @@
         <v>1</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="str">
         <v>N/A</v>
@@ -2518,28 +2518,28 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B61" t="str">
-        <v>rcervantes@live.com.mx</v>
+        <v>rsoberanis11@hotmail.com</v>
       </c>
       <c r="C61" t="str">
-        <v>RAÚL CERVANTES CEBALLOS</v>
+        <v>RICARDO ANTONIO SOBERANIS GAMBOA</v>
       </c>
       <c r="D61" t="str">
-        <v>9993382222</v>
+        <v>9993437376</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -2553,16 +2553,16 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B62" t="str">
-        <v>richfer0304@gmail.com</v>
+        <v>rcervantes@live.com.mx</v>
       </c>
       <c r="C62" t="str">
-        <v>RICARDO DANIEL FERNÁNDEZ PÉREZ</v>
+        <v>RAÚL CERVANTES CEBALLOS</v>
       </c>
       <c r="D62" t="str">
-        <v>999 163 9981</v>
+        <v>9993382222</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2588,19 +2588,19 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B63" t="str">
-        <v>richfer1020@gmail.com</v>
+        <v>richfer0304@gmail.com</v>
       </c>
       <c r="C63" t="str">
-        <v>RICARDO MANUEL FERNÁNDEZ QUIJANO</v>
+        <v>RICARDO DANIEL FERNÁNDEZ PÉREZ</v>
       </c>
       <c r="D63" t="str">
-        <v>999 947 3043</v>
+        <v>999 163 9981</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -2623,19 +2623,19 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B64" t="str">
-        <v>licyaelromero@gmail.com</v>
+        <v>richfer1020@gmail.com</v>
       </c>
       <c r="C64" t="str">
-        <v>YAEL ROMERO DE DIOS</v>
+        <v>RICARDO MANUEL FERNÁNDEZ QUIJANO</v>
       </c>
       <c r="D64" t="str">
-        <v>999 528 7779</v>
+        <v>999 947 3043</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2644,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -2658,16 +2658,16 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B65" t="str">
-        <v>aimeegomez615@gmail.com</v>
+        <v>licyaelromero@gmail.com</v>
       </c>
       <c r="C65" t="str">
-        <v>AIMEE GOMEZ MENDOZA</v>
+        <v>YAEL ROMERO DE DIOS</v>
       </c>
       <c r="D65" t="str">
-        <v>999 730 0081</v>
+        <v>999 528 7779</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2693,16 +2693,16 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B66" t="str">
-        <v>oso.guigam@gmail.com</v>
+        <v>aimeegomez615@gmail.com</v>
       </c>
       <c r="C66" t="str">
-        <v>LUIS FERNANDO GUILLERMO GAMBOA</v>
+        <v>AIMEE GOMEZ MENDOZA</v>
       </c>
       <c r="D66" t="str">
-        <v>9992420621</v>
+        <v>999 730 0081</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2728,28 +2728,28 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="B67" t="str">
-        <v>jacintolizarraga@hotmail.com</v>
+        <v>oso.guigam@gmail.com</v>
       </c>
       <c r="C67" t="str">
-        <v>JOSE JACINTO LIZARRAGA AVILA</v>
+        <v>LUIS FERNANDO GUILLERMO GAMBOA</v>
       </c>
       <c r="D67" t="str">
-        <v>9991336764</v>
+        <v>9992420621</v>
       </c>
       <c r="E67">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -2763,95 +2763,95 @@
     </row>
     <row r="68">
       <c r="A68">
+        <v>30</v>
+      </c>
+      <c r="B68" t="str">
+        <v>jacintolizarraga@hotmail.com</v>
+      </c>
+      <c r="C68" t="str">
+        <v>JOSE JACINTO LIZARRAGA AVILA</v>
+      </c>
+      <c r="D68" t="str">
+        <v>9991336764</v>
+      </c>
+      <c r="E68">
+        <v>5</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>3</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K68" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
         <v>31</v>
       </c>
-      <c r="B68" t="str">
+      <c r="B69" t="str">
         <v>fit.x66@hotmail.com</v>
       </c>
-      <c r="C68" t="str">
+      <c r="C69" t="str">
         <v>ADOLFO XACUR RIVERA</v>
       </c>
-      <c r="D68" t="str">
+      <c r="D69" t="str">
         <v>9992442613</v>
       </c>
-      <c r="E68">
+      <c r="E69">
         <v>8</v>
       </c>
-      <c r="F68">
-        <v>3</v>
-      </c>
-      <c r="G68">
-        <v>1</v>
-      </c>
-      <c r="H68">
-        <v>2</v>
-      </c>
-      <c r="I68">
-        <v>2</v>
-      </c>
-      <c r="J68" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K68" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
+      <c r="F69">
+        <v>3</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="J69" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K69" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
         <v>46</v>
       </c>
-      <c r="B69" t="str">
+      <c r="B70" t="str">
         <v>sysaventas@hotmail.com</v>
       </c>
-      <c r="C69" t="str">
+      <c r="C70" t="str">
         <v>REMIGIO BEETHOVEN AGUILAR CANTO</v>
       </c>
-      <c r="D69" t="str">
+      <c r="D70" t="str">
         <v>'9999238686</v>
       </c>
-      <c r="E69">
+      <c r="E70">
         <v>10</v>
       </c>
-      <c r="F69">
+      <c r="F70">
         <v>7</v>
       </c>
-      <c r="G69">
-        <v>3</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="J69" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K69" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70">
-        <v>51</v>
-      </c>
-      <c r="B70" t="str">
-        <v>manuel.chaidez@valledelsur.com.mx</v>
-      </c>
-      <c r="C70" t="str">
-        <v>MANUEL JESÚS CHAIDEZ PALACIOS</v>
-      </c>
-      <c r="D70" t="str">
-        <v>9992771732</v>
-      </c>
-      <c r="E70">
-        <v>5</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
       <c r="G70">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -2868,25 +2868,25 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B71" t="str">
-        <v>talleresmonforte@hotmail.com</v>
+        <v>manuel.chaidez@valledelsur.com.mx</v>
       </c>
       <c r="C71" t="str">
-        <v>PAULINO EDILBERTO MONFORTE TRAVA</v>
+        <v>MANUEL JESÚS CHAIDEZ PALACIOS</v>
       </c>
       <c r="D71" t="str">
-        <v>9999810995</v>
+        <v>9992771732</v>
       </c>
       <c r="E71">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F71">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -2903,28 +2903,28 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B72" t="str">
-        <v>recosadecv@prodigy.net.mx</v>
+        <v>talleresmonforte@hotmail.com</v>
       </c>
       <c r="C72" t="str">
-        <v>RIGOMAR HINOJOSA SHIELDS</v>
+        <v>PAULINO EDILBERTO MONFORTE TRAVA</v>
       </c>
       <c r="D72" t="str">
-        <v>9381200721</v>
+        <v>9999810995</v>
       </c>
       <c r="E72">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F72">
+        <v>3</v>
+      </c>
+      <c r="G72">
         <v>4</v>
       </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
       <c r="H72">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -2938,28 +2938,28 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B73" t="str">
-        <v>jordan910@hotmail.com</v>
+        <v>recosadecv@prodigy.net.mx</v>
       </c>
       <c r="C73" t="str">
-        <v>JUAN CARLOS JORDAN LOPEZ</v>
+        <v>RIGOMAR HINOJOSA SHIELDS</v>
       </c>
       <c r="D73" t="str">
-        <v>9999258499</v>
+        <v>9381200721</v>
       </c>
       <c r="E73">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F73">
         <v>4</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -2973,28 +2973,28 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B74" t="str">
-        <v>jorgedawn@prodigy.net.mx</v>
+        <v>jordan910@hotmail.com</v>
       </c>
       <c r="C74" t="str">
-        <v>JORGE ALFREDO DAWN MEDINA</v>
+        <v>JUAN CARLOS JORDAN LOPEZ</v>
       </c>
       <c r="D74" t="str">
-        <v>9999005153</v>
+        <v>9999258499</v>
       </c>
       <c r="E74">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G74">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -3008,31 +3008,31 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B75" t="str">
-        <v>ssg@santinelli.com.mx</v>
+        <v>jorgedawn@prodigy.net.mx</v>
       </c>
       <c r="C75" t="str">
-        <v>SERGIO SANTINELLI GRAJALES</v>
+        <v>JORGE ALFREDO DAWN MEDINA</v>
       </c>
       <c r="D75" t="str">
-        <v>5554388308</v>
+        <v>9999005153</v>
       </c>
       <c r="E75">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I75">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J75" t="str">
         <v>N/A</v>
@@ -3043,31 +3043,31 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B76" t="str">
-        <v>cc@secure.mx</v>
+        <v>ssg@santinelli.com.mx</v>
       </c>
       <c r="C76" t="str">
-        <v>CLAUDIO MAURICIO CANAVATI FARAH</v>
+        <v>SERGIO SANTINELLI GRAJALES</v>
       </c>
       <c r="D76" t="str">
-        <v>5554536965</v>
+        <v>5554388308</v>
       </c>
       <c r="E76">
         <v>8</v>
       </c>
       <c r="F76">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I76">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J76" t="str">
         <v>N/A</v>
@@ -3078,63 +3078,63 @@
     </row>
     <row r="77">
       <c r="A77">
+        <v>97</v>
+      </c>
+      <c r="B77" t="str">
+        <v>cc@secure.mx</v>
+      </c>
+      <c r="C77" t="str">
+        <v>CLAUDIO MAURICIO CANAVATI FARAH</v>
+      </c>
+      <c r="D77" t="str">
+        <v>5554536965</v>
+      </c>
+      <c r="E77">
+        <v>8</v>
+      </c>
+      <c r="F77">
+        <v>6</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="K77" t="str">
+        <v>Activo</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
         <v>99</v>
       </c>
-      <c r="B77" t="str">
+      <c r="B78" t="str">
         <v>al3xrivas@gmail.com</v>
       </c>
-      <c r="C77" t="str">
+      <c r="C78" t="str">
         <v>ALEJANDRO FRANCISCO RIVAS PINTADO</v>
       </c>
-      <c r="D77" t="str">
+      <c r="D78" t="str">
         <v>9997720959</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <v>4</v>
       </c>
-      <c r="F77">
-        <v>2</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>2</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="J77" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="K77" t="str">
-        <v>Activo</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="B78" t="str">
-        <v>rmadahuar@cotexsa.com.mx</v>
-      </c>
-      <c r="C78" t="str">
-        <v>ROBERTO JOSE MADAHUAR BOEHM</v>
-      </c>
-      <c r="D78" t="str">
-        <v>9999473478</v>
-      </c>
-      <c r="E78">
-        <v>2</v>
-      </c>
       <c r="F78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -3203,7 +3203,7 @@
         <v>Rifles:</v>
       </c>
       <c r="B8" t="str">
-        <v>09999470480999960026999933495759991637860999943155699610062889818296516999900127299920055509999490494999242905299994150529999494819'999238996199913358999992780476999947750199994791999992243874999297810399994779579991229424999240311055208696859991276042999137542799933560719991369874552098507399949920995530565722997124894099922475519991356502999151826699949128839901011913999145039955439006169993359825999532857055373400969811204947999394090998315490849999967145554342616044313029539993354270938152681199923150409993778311'999900136699957595429992003314+132134702709993772793999165084999934373769993382222999 163 9981999 947 3043999 528 7779999 730 0081999242062199913367649992442613'9999238686999277173299998109959381200721999925849999990051535554388308555453696599977209599999473478</v>
+        <v>099994704809999600269999334957599916378609999431556999947347899610062889818296516999900127299920055509999490494999242905299994150529999494819'999238996199913358999992780476999947750199994791999992243874999297810399994779579991229424999240311055208696859991276042999137542799933560719991369874552098507399949920995530565722997124894099922475519991356502999151826699949128839901011913999145039955439006169993359825999532857055373400969811204947999394090998315490849999967145554342616044313029539993354270938152681199923150409993778311'999900136699957595429992003314+132134702709993772793999165084999934373769993382222999 163 9981999 947 3043999 528 7779999 730 0081999242062199913367649992442613'999923868699927717329999810995938120072199992584999999005153555438830855545369659997720959</v>
       </c>
     </row>
     <row r="9">
@@ -3235,7 +3235,7 @@
         <v>Fecha Generación:</v>
       </c>
       <c r="B13" t="str">
-        <v>23/1/2026, 10:54:45 a.m.</v>
+        <v>23/1/2026, 11:00:52 a.m.</v>
       </c>
     </row>
     <row r="14">

</xml_diff>